<commit_message>
Add to Python Work space[23.07.24 21:48(T_01), by 진태만]
</commit_message>
<xml_diff>
--- a/dlk_airflow_01/l0/bi/01_L0BIM_DCT_CALENDAR.xlsx
+++ b/dlk_airflow_01/l0/bi/01_L0BIM_DCT_CALENDAR.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="현재_통합_문서" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ob_dsgn\L0BIM_DCT_CALENDAR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ob_dsgn\01_L0BIM_DCT_CALENDAR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20E9BC40-58E2-4432-A25E-0C0891B5781B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{09493AE2-93A2-4BED-B0E4-DF78E8C23341}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" tabRatio="949" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2640" yWindow="2640" windowWidth="28800" windowHeight="11295" tabRatio="949" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="T_01" sheetId="237" r:id="rId1"/>
@@ -41,7 +41,7 @@
     <t xml:space="preserve"> 배치 스케줄</t>
   </si>
   <si>
-    <t>1 2 • • ••</t>
+    <t>3 2 * * *</t>
     <phoneticPr fontId="37" type="noConversion"/>
   </si>
 </sst>
@@ -2076,7 +2076,7 @@
   <dimension ref="A1:K47"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>